<commit_message>
add dataframe for design_aspect and counts of criteria. remove duplicate operating cost.
</commit_message>
<xml_diff>
--- a/inst/extdata/Artificial Lift Matrix.xlsx
+++ b/inst/extdata/Artificial Lift Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\github-oilgains\artificial_lift_matrix\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430FC2CF-9B6C-4259-BC72-C6BF54E69AA2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B5A18A-9828-4799-9CB7-DD9EE9410C0B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="15" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
   <si>
     <t xml:space="preserve"> Design Aspect</t>
   </si>
@@ -342,9 +342,6 @@
   </si>
   <si>
     <t>&gt; 10 deg / 100'</t>
-  </si>
-  <si>
-    <t>Operating Cost</t>
   </si>
   <si>
     <t>Setup cost</t>
@@ -845,8 +842,8 @@
   </sheetPr>
   <dimension ref="A1:AL91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63:N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4309,10 +4306,10 @@
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="E62" s="10">
         <v>1</v>
@@ -4366,42 +4363,18 @@
     <row r="63" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E63" s="10">
-        <v>1</v>
-      </c>
-      <c r="F63" s="10">
-        <v>2</v>
-      </c>
-      <c r="G63" s="10">
-        <v>3</v>
-      </c>
-      <c r="H63" s="10">
-        <v>1</v>
-      </c>
-      <c r="I63" s="10">
-        <v>1</v>
-      </c>
-      <c r="J63" s="10">
-        <v>1</v>
-      </c>
-      <c r="K63" s="10">
-        <v>1</v>
-      </c>
-      <c r="L63" s="10">
-        <v>2</v>
-      </c>
-      <c r="M63" s="10">
-        <v>2</v>
-      </c>
-      <c r="N63" s="10">
-        <v>1</v>
-      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
+      <c r="N63" s="10"/>
       <c r="O63" s="10">
         <v>1</v>
       </c>

</xml_diff>